<commit_message>
remove description from test xlsx file.
</commit_message>
<xml_diff>
--- a/inst/extdata/matrix-input-slam.xlsx
+++ b/inst/extdata/matrix-input-slam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="O" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>variable</t>
   </si>
@@ -74,34 +74,19 @@
     <t>ch</t>
   </si>
   <si>
-    <t>Chassis</t>
-  </si>
-  <si>
     <t>&lt;=</t>
   </si>
   <si>
     <t>pt</t>
   </si>
   <si>
-    <t>Picture Tube</t>
-  </si>
-  <si>
     <t>sc</t>
   </si>
   <si>
-    <t>Speaker Cone</t>
-  </si>
-  <si>
     <t>ps</t>
   </si>
   <si>
-    <t>Power Supply</t>
-  </si>
-  <si>
     <t>el</t>
-  </si>
-  <si>
-    <t>Electronics</t>
   </si>
   <si>
     <t>i</t>
@@ -123,6 +108,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -633,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -646,13 +632,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -789,100 +775,81 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="D2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="C6">
         <v>600</v>
       </c>
     </row>

</xml_diff>